<commit_message>
final version of hashOpenAddressing
</commit_message>
<xml_diff>
--- a/aisd_lab_4_hash_table_open_adressing/open_addressing_note.xlsx
+++ b/aisd_lab_4_hash_table_open_adressing/open_addressing_note.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\materialy\III-sem\astruk\laby\lab01\astrukNauka\2021Z_AISD_lab_git_gr6\aisd_lab_4_hash_table_open_adressing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01951048-5132-46FB-B83D-819F4752D655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97EA8CC-AEA9-4F79-B108-50BF1E864FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1FE36D43-29F8-48E3-8A86-FBB2BB58C0A2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="21">
   <si>
     <t>Adresowanie liniowe:</t>
   </si>
@@ -88,6 +88,18 @@
   <si>
     <t>a = 10 b = 1</t>
   </si>
+  <si>
+    <t>WNIOSKI</t>
+  </si>
+  <si>
+    <t>1.  Dla adresowania liniowego widzimy, że początkowy rozmiar tablicy haszującej ma istotny wpływ na czas wstawiania do niej elementów. Jest on bardzo wysoki dla ilości elementów przekraczającej rozmiar tablicy haszującej. Dla początkowego rozmiaru hasza ponad dwukrotnie większego niż ilość elementów czas wstawiania jest już praktycznie identyczny z czasem szukania.</t>
+  </si>
+  <si>
+    <t>2. Dla adresowania podwójnego widzimy w porównaniu do adresowania liniowego dużo lepszy czas wstawiania elementów, a także szybszy czas szukania. Podobnie jak w adresowaniu liniowym widzimy dużą zmianę czas potrzebnego do wstawienia elementów, gdy początkowy rozmiar hasza jest ponad dwa razy większy niż liczba elementów do wstawienia.</t>
+  </si>
+  <si>
+    <t>3. Dla adresowania kwadratowego widzimy podobnie jak w poprzednich rodzajach adresowania - lepszy czas wstawiania dla początkowego rozmiaru tablicy większego niż liczba elementów do wstawienia. Nie widać zmiany czasu wstawiania i szukania dla różnych wartości a i b.</t>
+  </si>
 </sst>
 </file>
 
@@ -95,9 +107,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,6 +153,15 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -163,23 +184,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Dziesiętny" xfId="1" builtinId="3"/>
@@ -2676,10 +2703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32684610-2195-46AF-B216-FE019B525897}">
-  <dimension ref="A4:V60"/>
+  <dimension ref="A1:X60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14:X17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2688,21 +2715,71 @@
     <col min="2" max="2" width="8.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Q1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+    </row>
+    <row r="4" spans="1:24" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="Q4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -2715,162 +2792,264 @@
       <c r="D6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7">
         <v>512</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="1">
         <v>289</v>
       </c>
       <c r="D7">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8">
         <v>1024</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="1">
         <v>288</v>
       </c>
       <c r="D8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>3</v>
       </c>
       <c r="B9">
         <v>2048</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="1">
         <v>287</v>
       </c>
       <c r="D9">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="Q9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>4</v>
       </c>
       <c r="B10">
         <v>4096</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="1">
         <v>285</v>
       </c>
       <c r="D10">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>5</v>
       </c>
       <c r="B11">
         <v>8192</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="1">
         <v>285</v>
       </c>
       <c r="D11">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="9"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>6</v>
       </c>
       <c r="B12">
         <v>16384</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="1">
         <v>282</v>
       </c>
       <c r="D12">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>7</v>
       </c>
       <c r="B13">
         <v>32768</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="1">
         <v>277</v>
       </c>
       <c r="D13">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="9"/>
+      <c r="W13" s="9"/>
+      <c r="X13" s="9"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>8</v>
       </c>
       <c r="B14">
         <v>65536</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="1">
         <v>263</v>
       </c>
       <c r="D14">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="Q14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="9"/>
+      <c r="W14" s="9"/>
+      <c r="X14" s="9"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>9</v>
       </c>
       <c r="B15">
         <v>131072</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="1">
         <v>187</v>
       </c>
       <c r="D15">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="9"/>
+      <c r="W15" s="9"/>
+      <c r="X15" s="9"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>10</v>
       </c>
       <c r="B16">
         <v>262144</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="1">
         <v>5</v>
       </c>
       <c r="D16">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="9"/>
+      <c r="X17" s="9"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -2884,7 +3063,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1</v>
       </c>
@@ -2898,7 +3077,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2</v>
       </c>
@@ -2912,7 +3091,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2926,7 +3105,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>4</v>
       </c>
@@ -2940,7 +3119,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>5</v>
       </c>
@@ -2954,7 +3133,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>6</v>
       </c>
@@ -2968,7 +3147,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>7</v>
       </c>
@@ -2982,7 +3161,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>8</v>
       </c>
@@ -2996,7 +3175,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>9</v>
       </c>
@@ -3010,7 +3189,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>10</v>
       </c>
@@ -3025,120 +3204,120 @@
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
-      <c r="P34" s="4"/>
-      <c r="Q34" s="4"/>
-      <c r="R34" s="4"/>
-      <c r="S34" s="4"/>
-      <c r="T34" s="4"/>
-      <c r="U34" s="4"/>
-      <c r="V34" s="4"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+      <c r="S34" s="7"/>
+      <c r="T34" s="7"/>
+      <c r="U34" s="7"/>
+      <c r="V34" s="7"/>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-      <c r="P35" s="4"/>
-      <c r="Q35" s="4"/>
-      <c r="R35" s="4"/>
-      <c r="S35" s="4"/>
-      <c r="T35" s="4"/>
-      <c r="U35" s="4"/>
-      <c r="V35" s="4"/>
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="7"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+      <c r="S35" s="7"/>
+      <c r="T35" s="7"/>
+      <c r="U35" s="7"/>
+      <c r="V35" s="7"/>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-      <c r="P36" s="4"/>
-      <c r="Q36" s="4"/>
-      <c r="R36" s="4"/>
-      <c r="S36" s="4"/>
-      <c r="T36" s="4"/>
-      <c r="U36" s="4"/>
-      <c r="V36" s="4"/>
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+      <c r="S36" s="7"/>
+      <c r="T36" s="7"/>
+      <c r="U36" s="7"/>
+      <c r="V36" s="7"/>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1" t="s">
+      <c r="D37" s="4"/>
+      <c r="E37" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1" t="s">
+      <c r="F37" s="4"/>
+      <c r="G37" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1" t="s">
+      <c r="H37" s="4"/>
+      <c r="I37" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1" t="s">
+      <c r="J37" s="4"/>
+      <c r="K37" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1" t="s">
+      <c r="L37" s="4"/>
+      <c r="M37" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N37" s="1"/>
-      <c r="O37" s="1" t="s">
+      <c r="N37" s="4"/>
+      <c r="O37" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P37" s="1"/>
-      <c r="Q37" s="1" t="s">
+      <c r="P37" s="4"/>
+      <c r="Q37" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="R37" s="1"/>
-      <c r="S37" s="1" t="s">
+      <c r="R37" s="4"/>
+      <c r="S37" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="T37" s="1"/>
-      <c r="U37" s="1" t="s">
+      <c r="T37" s="4"/>
+      <c r="U37" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="V37" s="1"/>
+      <c r="V37" s="4"/>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
@@ -3215,64 +3394,64 @@
       <c r="B39">
         <v>512</v>
       </c>
-      <c r="C39" s="6">
+      <c r="C39" s="2">
         <v>17</v>
       </c>
-      <c r="D39" s="6">
-        <v>4</v>
-      </c>
-      <c r="E39" s="6">
+      <c r="D39" s="2">
+        <v>4</v>
+      </c>
+      <c r="E39" s="2">
         <v>16</v>
       </c>
-      <c r="F39" s="6">
-        <v>4</v>
-      </c>
-      <c r="G39" s="6">
+      <c r="F39" s="2">
+        <v>4</v>
+      </c>
+      <c r="G39" s="2">
         <v>15</v>
       </c>
-      <c r="H39" s="6">
-        <v>4</v>
-      </c>
-      <c r="I39" s="6">
+      <c r="H39" s="2">
+        <v>4</v>
+      </c>
+      <c r="I39" s="2">
         <v>15</v>
       </c>
-      <c r="J39" s="6">
-        <v>4</v>
-      </c>
-      <c r="K39" s="6">
+      <c r="J39" s="2">
+        <v>4</v>
+      </c>
+      <c r="K39" s="2">
         <v>15</v>
       </c>
-      <c r="L39" s="6">
-        <v>4</v>
-      </c>
-      <c r="M39" s="6">
+      <c r="L39" s="2">
+        <v>4</v>
+      </c>
+      <c r="M39" s="2">
         <v>15</v>
       </c>
-      <c r="N39" s="6">
-        <v>4</v>
-      </c>
-      <c r="O39" s="6">
+      <c r="N39" s="2">
+        <v>4</v>
+      </c>
+      <c r="O39" s="2">
         <v>15</v>
       </c>
-      <c r="P39" s="6">
-        <v>4</v>
-      </c>
-      <c r="Q39" s="6">
+      <c r="P39" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q39" s="2">
         <v>16</v>
       </c>
-      <c r="R39" s="6">
-        <v>4</v>
-      </c>
-      <c r="S39" s="6">
+      <c r="R39" s="2">
+        <v>4</v>
+      </c>
+      <c r="S39" s="2">
         <v>16</v>
       </c>
-      <c r="T39" s="6">
-        <v>4</v>
-      </c>
-      <c r="U39" s="6">
+      <c r="T39" s="2">
+        <v>4</v>
+      </c>
+      <c r="U39" s="2">
         <v>17</v>
       </c>
-      <c r="V39" s="6">
+      <c r="V39" s="2">
         <v>4</v>
       </c>
     </row>
@@ -3283,64 +3462,64 @@
       <c r="B40">
         <v>1024</v>
       </c>
-      <c r="C40" s="6">
+      <c r="C40" s="2">
         <v>15</v>
       </c>
-      <c r="D40" s="6">
-        <v>4</v>
-      </c>
-      <c r="E40" s="6">
+      <c r="D40" s="2">
+        <v>4</v>
+      </c>
+      <c r="E40" s="2">
         <v>15</v>
       </c>
-      <c r="F40" s="6">
-        <v>4</v>
-      </c>
-      <c r="G40" s="6">
+      <c r="F40" s="2">
+        <v>4</v>
+      </c>
+      <c r="G40" s="2">
         <v>14</v>
       </c>
-      <c r="H40" s="6">
-        <v>4</v>
-      </c>
-      <c r="I40" s="6">
+      <c r="H40" s="2">
+        <v>4</v>
+      </c>
+      <c r="I40" s="2">
         <v>15</v>
       </c>
-      <c r="J40" s="6">
-        <v>4</v>
-      </c>
-      <c r="K40" s="6">
+      <c r="J40" s="2">
+        <v>4</v>
+      </c>
+      <c r="K40" s="2">
         <v>15</v>
       </c>
-      <c r="L40" s="6">
-        <v>4</v>
-      </c>
-      <c r="M40" s="6">
+      <c r="L40" s="2">
+        <v>4</v>
+      </c>
+      <c r="M40" s="2">
         <v>15</v>
       </c>
-      <c r="N40" s="6">
-        <v>4</v>
-      </c>
-      <c r="O40" s="6">
+      <c r="N40" s="2">
+        <v>4</v>
+      </c>
+      <c r="O40" s="2">
         <v>15</v>
       </c>
-      <c r="P40" s="6">
-        <v>4</v>
-      </c>
-      <c r="Q40" s="6">
+      <c r="P40" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q40" s="2">
         <v>16</v>
       </c>
-      <c r="R40" s="6">
-        <v>4</v>
-      </c>
-      <c r="S40" s="6">
+      <c r="R40" s="2">
+        <v>4</v>
+      </c>
+      <c r="S40" s="2">
         <v>15</v>
       </c>
-      <c r="T40" s="6">
-        <v>4</v>
-      </c>
-      <c r="U40" s="6">
+      <c r="T40" s="2">
+        <v>4</v>
+      </c>
+      <c r="U40" s="2">
         <v>17</v>
       </c>
-      <c r="V40" s="6">
+      <c r="V40" s="2">
         <v>4</v>
       </c>
     </row>
@@ -3351,64 +3530,64 @@
       <c r="B41">
         <v>2048</v>
       </c>
-      <c r="C41" s="6">
+      <c r="C41" s="2">
         <v>15</v>
       </c>
-      <c r="D41" s="6">
-        <v>4</v>
-      </c>
-      <c r="E41" s="6">
+      <c r="D41" s="2">
+        <v>4</v>
+      </c>
+      <c r="E41" s="2">
         <v>15</v>
       </c>
-      <c r="F41" s="6">
-        <v>4</v>
-      </c>
-      <c r="G41" s="6">
+      <c r="F41" s="2">
+        <v>4</v>
+      </c>
+      <c r="G41" s="2">
         <v>15</v>
       </c>
-      <c r="H41" s="6">
-        <v>4</v>
-      </c>
-      <c r="I41" s="6">
+      <c r="H41" s="2">
+        <v>4</v>
+      </c>
+      <c r="I41" s="2">
         <v>15</v>
       </c>
-      <c r="J41" s="6">
-        <v>4</v>
-      </c>
-      <c r="K41" s="6">
+      <c r="J41" s="2">
+        <v>4</v>
+      </c>
+      <c r="K41" s="2">
         <v>14</v>
       </c>
-      <c r="L41" s="6">
-        <v>4</v>
-      </c>
-      <c r="M41" s="6">
+      <c r="L41" s="2">
+        <v>4</v>
+      </c>
+      <c r="M41" s="2">
         <v>15</v>
       </c>
-      <c r="N41" s="6">
-        <v>4</v>
-      </c>
-      <c r="O41" s="6">
+      <c r="N41" s="2">
+        <v>4</v>
+      </c>
+      <c r="O41" s="2">
         <v>15</v>
       </c>
-      <c r="P41" s="6">
-        <v>4</v>
-      </c>
-      <c r="Q41" s="6">
+      <c r="P41" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q41" s="2">
         <v>15</v>
       </c>
-      <c r="R41" s="6">
-        <v>4</v>
-      </c>
-      <c r="S41" s="6">
+      <c r="R41" s="2">
+        <v>4</v>
+      </c>
+      <c r="S41" s="2">
         <v>15</v>
       </c>
-      <c r="T41" s="6">
-        <v>4</v>
-      </c>
-      <c r="U41" s="6">
+      <c r="T41" s="2">
+        <v>4</v>
+      </c>
+      <c r="U41" s="2">
         <v>17</v>
       </c>
-      <c r="V41" s="6">
+      <c r="V41" s="2">
         <v>4</v>
       </c>
     </row>
@@ -3419,64 +3598,64 @@
       <c r="B42">
         <v>4096</v>
       </c>
-      <c r="C42" s="6">
+      <c r="C42" s="2">
         <v>15</v>
       </c>
-      <c r="D42" s="6">
-        <v>4</v>
-      </c>
-      <c r="E42" s="6">
+      <c r="D42" s="2">
+        <v>4</v>
+      </c>
+      <c r="E42" s="2">
         <v>15</v>
       </c>
-      <c r="F42" s="6">
-        <v>4</v>
-      </c>
-      <c r="G42" s="6">
+      <c r="F42" s="2">
+        <v>4</v>
+      </c>
+      <c r="G42" s="2">
         <v>14</v>
       </c>
-      <c r="H42" s="6">
-        <v>4</v>
-      </c>
-      <c r="I42" s="6">
+      <c r="H42" s="2">
+        <v>4</v>
+      </c>
+      <c r="I42" s="2">
         <v>15</v>
       </c>
-      <c r="J42" s="6">
-        <v>4</v>
-      </c>
-      <c r="K42" s="6">
+      <c r="J42" s="2">
+        <v>4</v>
+      </c>
+      <c r="K42" s="2">
         <v>15</v>
       </c>
-      <c r="L42" s="6">
-        <v>4</v>
-      </c>
-      <c r="M42" s="6">
+      <c r="L42" s="2">
+        <v>4</v>
+      </c>
+      <c r="M42" s="2">
         <v>15</v>
       </c>
-      <c r="N42" s="6">
-        <v>4</v>
-      </c>
-      <c r="O42" s="6">
+      <c r="N42" s="2">
+        <v>4</v>
+      </c>
+      <c r="O42" s="2">
         <v>15</v>
       </c>
-      <c r="P42" s="6">
-        <v>4</v>
-      </c>
-      <c r="Q42" s="6">
+      <c r="P42" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q42" s="2">
         <v>15</v>
       </c>
-      <c r="R42" s="6">
-        <v>4</v>
-      </c>
-      <c r="S42" s="6">
+      <c r="R42" s="2">
+        <v>4</v>
+      </c>
+      <c r="S42" s="2">
         <v>15</v>
       </c>
-      <c r="T42" s="6">
-        <v>4</v>
-      </c>
-      <c r="U42" s="6">
+      <c r="T42" s="2">
+        <v>4</v>
+      </c>
+      <c r="U42" s="2">
         <v>16</v>
       </c>
-      <c r="V42" s="6">
+      <c r="V42" s="2">
         <v>4</v>
       </c>
     </row>
@@ -3487,64 +3666,64 @@
       <c r="B43">
         <v>8192</v>
       </c>
-      <c r="C43" s="6">
+      <c r="C43" s="2">
         <v>15</v>
       </c>
-      <c r="D43" s="6">
-        <v>4</v>
-      </c>
-      <c r="E43" s="6">
+      <c r="D43" s="2">
+        <v>4</v>
+      </c>
+      <c r="E43" s="2">
         <v>15</v>
       </c>
-      <c r="F43" s="6">
-        <v>4</v>
-      </c>
-      <c r="G43" s="6">
+      <c r="F43" s="2">
+        <v>4</v>
+      </c>
+      <c r="G43" s="2">
         <v>14</v>
       </c>
-      <c r="H43" s="6">
-        <v>4</v>
-      </c>
-      <c r="I43" s="6">
+      <c r="H43" s="2">
+        <v>4</v>
+      </c>
+      <c r="I43" s="2">
         <v>14</v>
       </c>
-      <c r="J43" s="6">
-        <v>4</v>
-      </c>
-      <c r="K43" s="6">
+      <c r="J43" s="2">
+        <v>4</v>
+      </c>
+      <c r="K43" s="2">
         <v>14</v>
       </c>
-      <c r="L43" s="6">
-        <v>4</v>
-      </c>
-      <c r="M43" s="6">
+      <c r="L43" s="2">
+        <v>4</v>
+      </c>
+      <c r="M43" s="2">
         <v>15</v>
       </c>
-      <c r="N43" s="6">
-        <v>4</v>
-      </c>
-      <c r="O43" s="6">
+      <c r="N43" s="2">
+        <v>4</v>
+      </c>
+      <c r="O43" s="2">
         <v>15</v>
       </c>
-      <c r="P43" s="6">
-        <v>4</v>
-      </c>
-      <c r="Q43" s="6">
+      <c r="P43" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q43" s="2">
         <v>15</v>
       </c>
-      <c r="R43" s="6">
-        <v>4</v>
-      </c>
-      <c r="S43" s="6">
+      <c r="R43" s="2">
+        <v>4</v>
+      </c>
+      <c r="S43" s="2">
         <v>16</v>
       </c>
-      <c r="T43" s="6">
-        <v>4</v>
-      </c>
-      <c r="U43" s="6">
+      <c r="T43" s="2">
+        <v>4</v>
+      </c>
+      <c r="U43" s="2">
         <v>16</v>
       </c>
-      <c r="V43" s="6">
+      <c r="V43" s="2">
         <v>4</v>
       </c>
     </row>
@@ -3555,64 +3734,64 @@
       <c r="B44">
         <v>16384</v>
       </c>
-      <c r="C44" s="6">
+      <c r="C44" s="2">
         <v>15</v>
       </c>
-      <c r="D44" s="6">
-        <v>4</v>
-      </c>
-      <c r="E44" s="6">
+      <c r="D44" s="2">
+        <v>4</v>
+      </c>
+      <c r="E44" s="2">
         <v>15</v>
       </c>
-      <c r="F44" s="6">
-        <v>4</v>
-      </c>
-      <c r="G44" s="6">
+      <c r="F44" s="2">
+        <v>4</v>
+      </c>
+      <c r="G44" s="2">
         <v>14</v>
       </c>
-      <c r="H44" s="6">
-        <v>4</v>
-      </c>
-      <c r="I44" s="6">
+      <c r="H44" s="2">
+        <v>4</v>
+      </c>
+      <c r="I44" s="2">
         <v>14</v>
       </c>
-      <c r="J44" s="6">
-        <v>4</v>
-      </c>
-      <c r="K44" s="6">
+      <c r="J44" s="2">
+        <v>4</v>
+      </c>
+      <c r="K44" s="2">
         <v>14</v>
       </c>
-      <c r="L44" s="6">
-        <v>4</v>
-      </c>
-      <c r="M44" s="6">
+      <c r="L44" s="2">
+        <v>4</v>
+      </c>
+      <c r="M44" s="2">
         <v>15</v>
       </c>
-      <c r="N44" s="6">
-        <v>4</v>
-      </c>
-      <c r="O44" s="6">
+      <c r="N44" s="2">
+        <v>4</v>
+      </c>
+      <c r="O44" s="2">
         <v>14</v>
       </c>
-      <c r="P44" s="6">
-        <v>4</v>
-      </c>
-      <c r="Q44" s="6">
+      <c r="P44" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q44" s="2">
         <v>15</v>
       </c>
-      <c r="R44" s="6">
-        <v>4</v>
-      </c>
-      <c r="S44" s="6">
+      <c r="R44" s="2">
+        <v>4</v>
+      </c>
+      <c r="S44" s="2">
         <v>15</v>
       </c>
-      <c r="T44" s="6">
-        <v>4</v>
-      </c>
-      <c r="U44" s="6">
+      <c r="T44" s="2">
+        <v>4</v>
+      </c>
+      <c r="U44" s="2">
         <v>16</v>
       </c>
-      <c r="V44" s="6">
+      <c r="V44" s="2">
         <v>4</v>
       </c>
     </row>
@@ -3623,64 +3802,64 @@
       <c r="B45">
         <v>32768</v>
       </c>
-      <c r="C45" s="6">
+      <c r="C45" s="2">
         <v>14</v>
       </c>
-      <c r="D45" s="6">
-        <v>4</v>
-      </c>
-      <c r="E45" s="6">
+      <c r="D45" s="2">
+        <v>4</v>
+      </c>
+      <c r="E45" s="2">
         <v>15</v>
       </c>
-      <c r="F45" s="6">
-        <v>4</v>
-      </c>
-      <c r="G45" s="6">
+      <c r="F45" s="2">
+        <v>4</v>
+      </c>
+      <c r="G45" s="2">
         <v>14</v>
       </c>
-      <c r="H45" s="6">
-        <v>4</v>
-      </c>
-      <c r="I45" s="6">
+      <c r="H45" s="2">
+        <v>4</v>
+      </c>
+      <c r="I45" s="2">
         <v>13</v>
       </c>
-      <c r="J45" s="6">
-        <v>4</v>
-      </c>
-      <c r="K45" s="6">
+      <c r="J45" s="2">
+        <v>4</v>
+      </c>
+      <c r="K45" s="2">
         <v>14</v>
       </c>
-      <c r="L45" s="6">
-        <v>4</v>
-      </c>
-      <c r="M45" s="6">
+      <c r="L45" s="2">
+        <v>4</v>
+      </c>
+      <c r="M45" s="2">
         <v>14</v>
       </c>
-      <c r="N45" s="6">
-        <v>4</v>
-      </c>
-      <c r="O45" s="6">
+      <c r="N45" s="2">
+        <v>4</v>
+      </c>
+      <c r="O45" s="2">
         <v>14</v>
       </c>
-      <c r="P45" s="6">
-        <v>4</v>
-      </c>
-      <c r="Q45" s="6">
+      <c r="P45" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q45" s="2">
         <v>14</v>
       </c>
-      <c r="R45" s="6">
-        <v>4</v>
-      </c>
-      <c r="S45" s="6">
+      <c r="R45" s="2">
+        <v>4</v>
+      </c>
+      <c r="S45" s="2">
         <v>15</v>
       </c>
-      <c r="T45" s="6">
-        <v>4</v>
-      </c>
-      <c r="U45" s="6">
+      <c r="T45" s="2">
+        <v>4</v>
+      </c>
+      <c r="U45" s="2">
         <v>15</v>
       </c>
-      <c r="V45" s="6">
+      <c r="V45" s="2">
         <v>4</v>
       </c>
     </row>
@@ -3691,64 +3870,64 @@
       <c r="B46">
         <v>65536</v>
       </c>
-      <c r="C46" s="6">
+      <c r="C46" s="2">
         <v>13</v>
       </c>
-      <c r="D46" s="6">
-        <v>4</v>
-      </c>
-      <c r="E46" s="6">
+      <c r="D46" s="2">
+        <v>4</v>
+      </c>
+      <c r="E46" s="2">
         <v>16</v>
       </c>
-      <c r="F46" s="6">
-        <v>4</v>
-      </c>
-      <c r="G46" s="6">
+      <c r="F46" s="2">
+        <v>4</v>
+      </c>
+      <c r="G46" s="2">
         <v>13</v>
       </c>
-      <c r="H46" s="6">
-        <v>4</v>
-      </c>
-      <c r="I46" s="6">
+      <c r="H46" s="2">
+        <v>4</v>
+      </c>
+      <c r="I46" s="2">
         <v>13</v>
       </c>
-      <c r="J46" s="6">
-        <v>4</v>
-      </c>
-      <c r="K46" s="6">
+      <c r="J46" s="2">
+        <v>4</v>
+      </c>
+      <c r="K46" s="2">
         <v>13</v>
       </c>
-      <c r="L46" s="6">
-        <v>4</v>
-      </c>
-      <c r="M46" s="6">
+      <c r="L46" s="2">
+        <v>4</v>
+      </c>
+      <c r="M46" s="2">
         <v>13</v>
       </c>
-      <c r="N46" s="6">
-        <v>4</v>
-      </c>
-      <c r="O46" s="6">
+      <c r="N46" s="2">
+        <v>4</v>
+      </c>
+      <c r="O46" s="2">
         <v>13</v>
       </c>
-      <c r="P46" s="6">
-        <v>4</v>
-      </c>
-      <c r="Q46" s="6">
+      <c r="P46" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q46" s="2">
         <v>13</v>
       </c>
-      <c r="R46" s="6">
-        <v>4</v>
-      </c>
-      <c r="S46" s="6">
+      <c r="R46" s="2">
+        <v>4</v>
+      </c>
+      <c r="S46" s="2">
         <v>14</v>
       </c>
-      <c r="T46" s="6">
-        <v>4</v>
-      </c>
-      <c r="U46" s="6">
+      <c r="T46" s="2">
+        <v>4</v>
+      </c>
+      <c r="U46" s="2">
         <v>14</v>
       </c>
-      <c r="V46" s="6">
+      <c r="V46" s="2">
         <v>4</v>
       </c>
     </row>
@@ -3759,64 +3938,64 @@
       <c r="B47">
         <v>131072</v>
       </c>
-      <c r="C47" s="6">
+      <c r="C47" s="2">
         <v>11</v>
       </c>
-      <c r="D47" s="6">
-        <v>4</v>
-      </c>
-      <c r="E47" s="6">
+      <c r="D47" s="2">
+        <v>4</v>
+      </c>
+      <c r="E47" s="2">
         <v>11</v>
       </c>
-      <c r="F47" s="6">
-        <v>4</v>
-      </c>
-      <c r="G47" s="6">
+      <c r="F47" s="2">
+        <v>4</v>
+      </c>
+      <c r="G47" s="2">
         <v>11</v>
       </c>
-      <c r="H47" s="6">
-        <v>4</v>
-      </c>
-      <c r="I47" s="6">
+      <c r="H47" s="2">
+        <v>4</v>
+      </c>
+      <c r="I47" s="2">
         <v>11</v>
       </c>
-      <c r="J47" s="6">
-        <v>4</v>
-      </c>
-      <c r="K47" s="6">
+      <c r="J47" s="2">
+        <v>4</v>
+      </c>
+      <c r="K47" s="2">
         <v>11</v>
       </c>
-      <c r="L47" s="6">
-        <v>4</v>
-      </c>
-      <c r="M47" s="6">
+      <c r="L47" s="2">
+        <v>4</v>
+      </c>
+      <c r="M47" s="2">
         <v>11</v>
       </c>
-      <c r="N47" s="6">
-        <v>4</v>
-      </c>
-      <c r="O47" s="6">
+      <c r="N47" s="2">
+        <v>4</v>
+      </c>
+      <c r="O47" s="2">
         <v>11</v>
       </c>
-      <c r="P47" s="6">
-        <v>4</v>
-      </c>
-      <c r="Q47" s="6">
+      <c r="P47" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q47" s="2">
         <v>11</v>
       </c>
-      <c r="R47" s="6">
-        <v>4</v>
-      </c>
-      <c r="S47" s="6">
+      <c r="R47" s="2">
+        <v>4</v>
+      </c>
+      <c r="S47" s="2">
         <v>12</v>
       </c>
-      <c r="T47" s="6">
-        <v>4</v>
-      </c>
-      <c r="U47" s="6">
+      <c r="T47" s="2">
+        <v>4</v>
+      </c>
+      <c r="U47" s="2">
         <v>12</v>
       </c>
-      <c r="V47" s="6">
+      <c r="V47" s="2">
         <v>4</v>
       </c>
     </row>
@@ -3827,294 +4006,293 @@
       <c r="B48">
         <v>262144</v>
       </c>
-      <c r="C48" s="6">
-        <v>4</v>
-      </c>
-      <c r="D48" s="6">
+      <c r="C48" s="2">
+        <v>4</v>
+      </c>
+      <c r="D48" s="2">
         <v>3</v>
       </c>
-      <c r="E48" s="6">
-        <v>4</v>
-      </c>
-      <c r="F48" s="6">
-        <v>4</v>
-      </c>
-      <c r="G48" s="6">
-        <v>4</v>
-      </c>
-      <c r="H48" s="6">
+      <c r="E48" s="2">
+        <v>4</v>
+      </c>
+      <c r="F48" s="2">
+        <v>4</v>
+      </c>
+      <c r="G48" s="2">
+        <v>4</v>
+      </c>
+      <c r="H48" s="2">
         <v>3</v>
       </c>
-      <c r="I48" s="6">
-        <v>4</v>
-      </c>
-      <c r="J48" s="6">
+      <c r="I48" s="2">
+        <v>4</v>
+      </c>
+      <c r="J48" s="2">
         <v>3</v>
       </c>
-      <c r="K48" s="6">
-        <v>4</v>
-      </c>
-      <c r="L48" s="6">
+      <c r="K48" s="2">
+        <v>4</v>
+      </c>
+      <c r="L48" s="2">
         <v>3</v>
       </c>
-      <c r="M48" s="6">
-        <v>4</v>
-      </c>
-      <c r="N48" s="6">
+      <c r="M48" s="2">
+        <v>4</v>
+      </c>
+      <c r="N48" s="2">
         <v>3</v>
       </c>
-      <c r="O48" s="6">
-        <v>4</v>
-      </c>
-      <c r="P48" s="6">
+      <c r="O48" s="2">
+        <v>4</v>
+      </c>
+      <c r="P48" s="2">
         <v>3</v>
       </c>
-      <c r="Q48" s="6">
-        <v>4</v>
-      </c>
-      <c r="R48" s="6">
+      <c r="Q48" s="2">
+        <v>4</v>
+      </c>
+      <c r="R48" s="2">
         <v>3</v>
       </c>
-      <c r="S48" s="6">
-        <v>4</v>
-      </c>
-      <c r="T48" s="6">
+      <c r="S48" s="2">
+        <v>4</v>
+      </c>
+      <c r="T48" s="2">
         <v>3</v>
       </c>
-      <c r="U48" s="6">
-        <v>4</v>
-      </c>
-      <c r="V48" s="6">
+      <c r="U48" s="2">
+        <v>4</v>
+      </c>
+      <c r="V48" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="51" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C51" s="7"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="7"/>
-      <c r="G51" s="7"/>
-      <c r="H51" s="7"/>
-      <c r="I51" s="7"/>
-      <c r="J51" s="7"/>
-      <c r="K51" s="7"/>
-      <c r="L51" s="7"/>
-      <c r="M51" s="7"/>
-      <c r="N51" s="7"/>
-      <c r="O51" s="7"/>
-      <c r="P51" s="7"/>
-      <c r="Q51" s="7"/>
-      <c r="R51" s="7"/>
-      <c r="S51" s="7"/>
-      <c r="T51" s="7"/>
-      <c r="U51" s="7"/>
-      <c r="V51" s="7"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3"/>
+      <c r="N51" s="3"/>
+      <c r="O51" s="3"/>
+      <c r="P51" s="3"/>
+      <c r="Q51" s="3"/>
+      <c r="R51" s="3"/>
+      <c r="S51" s="3"/>
+      <c r="T51" s="3"/>
+      <c r="U51" s="3"/>
+      <c r="V51" s="3"/>
     </row>
     <row r="52" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="7"/>
-      <c r="F52" s="7"/>
-      <c r="G52" s="7"/>
-      <c r="H52" s="7"/>
-      <c r="I52" s="7"/>
-      <c r="J52" s="7"/>
-      <c r="K52" s="7"/>
-      <c r="L52" s="7"/>
-      <c r="M52" s="7"/>
-      <c r="N52" s="7"/>
-      <c r="O52" s="7"/>
-      <c r="P52" s="7"/>
-      <c r="Q52" s="7"/>
-      <c r="R52" s="7"/>
-      <c r="S52" s="7"/>
-      <c r="T52" s="7"/>
-      <c r="U52" s="7"/>
-      <c r="V52" s="7"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3"/>
+      <c r="N52" s="3"/>
+      <c r="O52" s="3"/>
+      <c r="P52" s="3"/>
+      <c r="Q52" s="3"/>
+      <c r="R52" s="3"/>
+      <c r="S52" s="3"/>
+      <c r="T52" s="3"/>
+      <c r="U52" s="3"/>
+      <c r="V52" s="3"/>
     </row>
     <row r="53" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="7"/>
-      <c r="G53" s="7"/>
-      <c r="H53" s="7"/>
-      <c r="I53" s="7"/>
-      <c r="J53" s="7"/>
-      <c r="K53" s="7"/>
-      <c r="L53" s="7"/>
-      <c r="M53" s="7"/>
-      <c r="N53" s="7"/>
-      <c r="O53" s="7"/>
-      <c r="P53" s="7"/>
-      <c r="Q53" s="7"/>
-      <c r="R53" s="7"/>
-      <c r="S53" s="7"/>
-      <c r="T53" s="7"/>
-      <c r="U53" s="7"/>
-      <c r="V53" s="7"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="3"/>
+      <c r="L53" s="3"/>
+      <c r="M53" s="3"/>
+      <c r="N53" s="3"/>
+      <c r="O53" s="3"/>
+      <c r="P53" s="3"/>
+      <c r="Q53" s="3"/>
+      <c r="R53" s="3"/>
+      <c r="S53" s="3"/>
+      <c r="T53" s="3"/>
+      <c r="U53" s="3"/>
+      <c r="V53" s="3"/>
     </row>
     <row r="54" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C54" s="7"/>
-      <c r="D54" s="7"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="7"/>
-      <c r="G54" s="7"/>
-      <c r="H54" s="7"/>
-      <c r="I54" s="7"/>
-      <c r="J54" s="7"/>
-      <c r="K54" s="7"/>
-      <c r="L54" s="7"/>
-      <c r="M54" s="7"/>
-      <c r="N54" s="7"/>
-      <c r="O54" s="7"/>
-      <c r="P54" s="7"/>
-      <c r="Q54" s="7"/>
-      <c r="R54" s="7"/>
-      <c r="S54" s="7"/>
-      <c r="T54" s="7"/>
-      <c r="U54" s="7"/>
-      <c r="V54" s="7"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+      <c r="I54" s="3"/>
+      <c r="J54" s="3"/>
+      <c r="K54" s="3"/>
+      <c r="L54" s="3"/>
+      <c r="M54" s="3"/>
+      <c r="N54" s="3"/>
+      <c r="O54" s="3"/>
+      <c r="P54" s="3"/>
+      <c r="Q54" s="3"/>
+      <c r="R54" s="3"/>
+      <c r="S54" s="3"/>
+      <c r="T54" s="3"/>
+      <c r="U54" s="3"/>
+      <c r="V54" s="3"/>
     </row>
     <row r="55" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C55" s="7"/>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
-      <c r="G55" s="7"/>
-      <c r="H55" s="7"/>
-      <c r="I55" s="7"/>
-      <c r="J55" s="7"/>
-      <c r="K55" s="7"/>
-      <c r="L55" s="7"/>
-      <c r="M55" s="7"/>
-      <c r="N55" s="7"/>
-      <c r="O55" s="7"/>
-      <c r="P55" s="7"/>
-      <c r="Q55" s="7"/>
-      <c r="R55" s="7"/>
-      <c r="S55" s="7"/>
-      <c r="T55" s="7"/>
-      <c r="U55" s="7"/>
-      <c r="V55" s="7"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
+      <c r="K55" s="3"/>
+      <c r="L55" s="3"/>
+      <c r="M55" s="3"/>
+      <c r="N55" s="3"/>
+      <c r="O55" s="3"/>
+      <c r="P55" s="3"/>
+      <c r="Q55" s="3"/>
+      <c r="R55" s="3"/>
+      <c r="S55" s="3"/>
+      <c r="T55" s="3"/>
+      <c r="U55" s="3"/>
+      <c r="V55" s="3"/>
     </row>
     <row r="56" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C56" s="7"/>
-      <c r="D56" s="7"/>
-      <c r="E56" s="7"/>
-      <c r="F56" s="7"/>
-      <c r="G56" s="7"/>
-      <c r="H56" s="7"/>
-      <c r="I56" s="7"/>
-      <c r="J56" s="7"/>
-      <c r="K56" s="7"/>
-      <c r="L56" s="7"/>
-      <c r="M56" s="7"/>
-      <c r="N56" s="7"/>
-      <c r="O56" s="7"/>
-      <c r="P56" s="7"/>
-      <c r="Q56" s="7"/>
-      <c r="R56" s="7"/>
-      <c r="S56" s="7"/>
-      <c r="T56" s="7"/>
-      <c r="U56" s="7"/>
-      <c r="V56" s="7"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
+      <c r="K56" s="3"/>
+      <c r="L56" s="3"/>
+      <c r="M56" s="3"/>
+      <c r="N56" s="3"/>
+      <c r="O56" s="3"/>
+      <c r="P56" s="3"/>
+      <c r="Q56" s="3"/>
+      <c r="R56" s="3"/>
+      <c r="S56" s="3"/>
+      <c r="T56" s="3"/>
+      <c r="U56" s="3"/>
+      <c r="V56" s="3"/>
     </row>
     <row r="57" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C57" s="7"/>
-      <c r="D57" s="7"/>
-      <c r="E57" s="7"/>
-      <c r="F57" s="7"/>
-      <c r="G57" s="7"/>
-      <c r="H57" s="7"/>
-      <c r="I57" s="7"/>
-      <c r="J57" s="7"/>
-      <c r="K57" s="7"/>
-      <c r="L57" s="7"/>
-      <c r="M57" s="7"/>
-      <c r="N57" s="7"/>
-      <c r="O57" s="7"/>
-      <c r="P57" s="7"/>
-      <c r="Q57" s="7"/>
-      <c r="R57" s="7"/>
-      <c r="S57" s="7"/>
-      <c r="T57" s="7"/>
-      <c r="U57" s="7"/>
-      <c r="V57" s="7"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="3"/>
+      <c r="J57" s="3"/>
+      <c r="K57" s="3"/>
+      <c r="L57" s="3"/>
+      <c r="M57" s="3"/>
+      <c r="N57" s="3"/>
+      <c r="O57" s="3"/>
+      <c r="P57" s="3"/>
+      <c r="Q57" s="3"/>
+      <c r="R57" s="3"/>
+      <c r="S57" s="3"/>
+      <c r="T57" s="3"/>
+      <c r="U57" s="3"/>
+      <c r="V57" s="3"/>
     </row>
     <row r="58" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C58" s="7"/>
-      <c r="D58" s="7"/>
-      <c r="E58" s="7"/>
-      <c r="F58" s="7"/>
-      <c r="G58" s="7"/>
-      <c r="H58" s="7"/>
-      <c r="I58" s="7"/>
-      <c r="J58" s="7"/>
-      <c r="K58" s="7"/>
-      <c r="L58" s="7"/>
-      <c r="M58" s="7"/>
-      <c r="N58" s="7"/>
-      <c r="O58" s="7"/>
-      <c r="P58" s="7"/>
-      <c r="Q58" s="7"/>
-      <c r="R58" s="7"/>
-      <c r="S58" s="7"/>
-      <c r="T58" s="7"/>
-      <c r="U58" s="7"/>
-      <c r="V58" s="7"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
+      <c r="I58" s="3"/>
+      <c r="J58" s="3"/>
+      <c r="K58" s="3"/>
+      <c r="L58" s="3"/>
+      <c r="M58" s="3"/>
+      <c r="N58" s="3"/>
+      <c r="O58" s="3"/>
+      <c r="P58" s="3"/>
+      <c r="Q58" s="3"/>
+      <c r="R58" s="3"/>
+      <c r="S58" s="3"/>
+      <c r="T58" s="3"/>
+      <c r="U58" s="3"/>
+      <c r="V58" s="3"/>
     </row>
     <row r="59" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C59" s="7"/>
-      <c r="D59" s="7"/>
-      <c r="E59" s="7"/>
-      <c r="F59" s="7"/>
-      <c r="G59" s="7"/>
-      <c r="H59" s="7"/>
-      <c r="I59" s="7"/>
-      <c r="J59" s="7"/>
-      <c r="K59" s="7"/>
-      <c r="L59" s="7"/>
-      <c r="M59" s="7"/>
-      <c r="N59" s="7"/>
-      <c r="O59" s="7"/>
-      <c r="P59" s="7"/>
-      <c r="Q59" s="7"/>
-      <c r="R59" s="7"/>
-      <c r="S59" s="7"/>
-      <c r="T59" s="7"/>
-      <c r="U59" s="7"/>
-      <c r="V59" s="7"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="3"/>
+      <c r="J59" s="3"/>
+      <c r="K59" s="3"/>
+      <c r="L59" s="3"/>
+      <c r="M59" s="3"/>
+      <c r="N59" s="3"/>
+      <c r="O59" s="3"/>
+      <c r="P59" s="3"/>
+      <c r="Q59" s="3"/>
+      <c r="R59" s="3"/>
+      <c r="S59" s="3"/>
+      <c r="T59" s="3"/>
+      <c r="U59" s="3"/>
+      <c r="V59" s="3"/>
     </row>
     <row r="60" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C60" s="7"/>
-      <c r="D60" s="7"/>
-      <c r="E60" s="7"/>
-      <c r="F60" s="7"/>
-      <c r="G60" s="7"/>
-      <c r="H60" s="7"/>
-      <c r="I60" s="7"/>
-      <c r="J60" s="7"/>
-      <c r="K60" s="7"/>
-      <c r="L60" s="7"/>
-      <c r="M60" s="7"/>
-      <c r="N60" s="7"/>
-      <c r="O60" s="7"/>
-      <c r="P60" s="7"/>
-      <c r="Q60" s="7"/>
-      <c r="R60" s="7"/>
-      <c r="S60" s="7"/>
-      <c r="T60" s="7"/>
-      <c r="U60" s="7"/>
-      <c r="V60" s="7"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="3"/>
+      <c r="J60" s="3"/>
+      <c r="K60" s="3"/>
+      <c r="L60" s="3"/>
+      <c r="M60" s="3"/>
+      <c r="N60" s="3"/>
+      <c r="O60" s="3"/>
+      <c r="P60" s="3"/>
+      <c r="Q60" s="3"/>
+      <c r="R60" s="3"/>
+      <c r="S60" s="3"/>
+      <c r="T60" s="3"/>
+      <c r="U60" s="3"/>
+      <c r="V60" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="O37:P37"/>
-    <mergeCell ref="Q37:R37"/>
-    <mergeCell ref="S37:T37"/>
+  <mergeCells count="17">
+    <mergeCell ref="Q1:X3"/>
+    <mergeCell ref="Q4:X8"/>
+    <mergeCell ref="Q9:X13"/>
+    <mergeCell ref="Q14:X17"/>
     <mergeCell ref="U37:V37"/>
     <mergeCell ref="A4:D5"/>
     <mergeCell ref="A20:D21"/>
@@ -4123,6 +4301,11 @@
     <mergeCell ref="G37:H37"/>
     <mergeCell ref="I37:J37"/>
     <mergeCell ref="A34:V36"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="O37:P37"/>
+    <mergeCell ref="Q37:R37"/>
+    <mergeCell ref="S37:T37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>